<commit_message>
Added Exceluse with application
</commit_message>
<xml_diff>
--- a/bin/dataprovider.xlsx
+++ b/bin/dataprovider.xlsx
@@ -3,20 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.maiya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.maiya\workspace\Selenium_03_2018\NewSelenium_Updated\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="2925"/>
   </bookViews>
   <sheets>
     <sheet name="Reg_page" sheetId="1" r:id="rId1"/>
+    <sheet name="marvel" r:id="rId5" sheetId="2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>firstname</t>
   </si>
@@ -41,25 +42,56 @@
     <t>password</t>
   </si>
   <si>
-    <t>sandesh</t>
-  </si>
-  <si>
     <t>matters</t>
   </si>
   <si>
     <t>sandesh.matters@gmail.com</t>
   </si>
   <si>
-    <t>s.matter</t>
-  </si>
-  <si>
     <t>sandesh1</t>
+  </si>
+  <si>
+    <t>smatter</t>
+  </si>
+  <si>
+    <t>Sandesh</t>
+  </si>
+  <si>
+    <t>Suhas</t>
+  </si>
+  <si>
+    <t>sumatters</t>
+  </si>
+  <si>
+    <t>suhas2</t>
+  </si>
+  <si>
+    <t>Gopi</t>
+  </si>
+  <si>
+    <t>gmatters</t>
+  </si>
+  <si>
+    <t>gopi01</t>
+  </si>
+  <si>
+    <t>Suhas.matters@gmail.com</t>
+  </si>
+  <si>
+    <t>Gopi.matters@gmail.com</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +120,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -103,11 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,16 +427,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -413,26 +456,104 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in Excel code
</commit_message>
<xml_diff>
--- a/bin/dataprovider.xlsx
+++ b/bin/dataprovider.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Reg_page" sheetId="1" r:id="rId1"/>
     <sheet name="WebTable" sheetId="2" r:id="rId2"/>
+    <sheet name="newSheet" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>firstname</t>
   </si>
@@ -172,7 +173,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +188,186 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor indexed="55"/>
       </patternFill>
     </fill>
@@ -208,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,6 +397,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +822,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD1048576"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,7 +843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -655,7 +854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -666,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -677,7 +876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -688,7 +887,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -699,7 +898,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -713,4 +912,73 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s" s="14">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s" s="15">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s" s="17">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s" s="18">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s" s="19">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s" s="20">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s" s="22">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>